<commit_message>
truven claim details counting done
</commit_message>
<xml_diff>
--- a/greenplum/datawarehouse/QA/qa-all-db-checks/truven/dw_staging/outputs/truven-claim-details-counting.xlsx
+++ b/greenplum/datawarehouse/QA/qa-all-db-checks/truven/dw_staging/outputs/truven-claim-details-counting.xlsx
@@ -6,18 +6,19 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="claim-details" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="distinct-claim-ids" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="distinct-enrolid-clmid-combos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t xml:space="preserve">Count of distinct claim IDs (msclmid) in data_warehouse and Truven schema on TACC server</t>
   </si>
   <si>
-    <t xml:space="preserve">Run time: 2023-01-05 17:06:14</t>
+    <t xml:space="preserve">Run time: 2023-01-10 14:26:17</t>
   </si>
   <si>
     <t xml:space="preserve">year</t>
@@ -119,18 +120,6 @@
     <t xml:space="preserve">18332458</t>
   </si>
   <si>
-    <t xml:space="preserve">7236327</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36487140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3849715</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18333150</t>
-  </si>
-  <si>
     <t xml:space="preserve">6715083</t>
   </si>
   <si>
@@ -143,18 +132,6 @@
     <t xml:space="preserve">16275643</t>
   </si>
   <si>
-    <t xml:space="preserve">6724984</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37550070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2960170</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16276747</t>
-  </si>
-  <si>
     <t xml:space="preserve">7498614</t>
   </si>
   <si>
@@ -167,18 +144,6 @@
     <t xml:space="preserve">12651429</t>
   </si>
   <si>
-    <t xml:space="preserve">7508331</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50229030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1993365</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12652141</t>
-  </si>
-  <si>
     <t xml:space="preserve">6912682</t>
   </si>
   <si>
@@ -191,18 +156,6 @@
     <t xml:space="preserve">13362344</t>
   </si>
   <si>
-    <t xml:space="preserve">6920009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43892681</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1966388</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13363141</t>
-  </si>
-  <si>
     <t xml:space="preserve">6885963</t>
   </si>
   <si>
@@ -215,40 +168,28 @@
     <t xml:space="preserve">17636955</t>
   </si>
   <si>
-    <t xml:space="preserve">6892886</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46332613</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3092110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17638717</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1461270</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25623813</t>
-  </si>
-  <si>
-    <t xml:space="preserve">538628</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4327923</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6517441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43596836</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3265479</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16447223</t>
+    <t xml:space="preserve">6502128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43595228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3264925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16446561</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6512965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43595978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3265064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16446722</t>
   </si>
   <si>
     <t xml:space="preserve">Difference between Truven schema and data_warehouse (Truven - DW):</t>
@@ -269,76 +210,220 @@
     <t xml:space="preserve">0</t>
   </si>
   <si>
-    <t xml:space="preserve">10598</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12837</t>
-  </si>
-  <si>
-    <t xml:space="preserve">577</t>
-  </si>
-  <si>
-    <t xml:space="preserve">692</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9901</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14955</t>
-  </si>
-  <si>
-    <t xml:space="preserve">592</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9717</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8922</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230</t>
-  </si>
-  <si>
-    <t xml:space="preserve">712</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7327</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5262</t>
-  </si>
-  <si>
-    <t xml:space="preserve">94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">797</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6923</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7653</t>
-  </si>
-  <si>
-    <t xml:space="preserve">516</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1762</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5056171</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17973023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2726851</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12119300</t>
+    <t xml:space="preserve">10837</t>
+  </si>
+  <si>
+    <t xml:space="preserve">750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: The difference in claim id count in 2021 is because some claims have enrolids that exist in the s and o tables that do not map to any enrolid in the a or t tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The reason that this discrepancy ONLY exists in 2021 is likely because for 2020 and earlier, Will created entries in dim_uth_member_id to accomodate them</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of distinct enrolid-clmid combinations in data_warehouse and Truven schema on TACC server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run time: 2023-01-10 14:26:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw_concat_ccaes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw_concat_ccaeo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw_concat_mdcrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dw_concat_mdcro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">truv_concat_ccaes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">truv_concat_ccaeo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">truv_concat_mdcrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">truv_concat_mdcro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22342712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">465722230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10836749</t>
+  </si>
+  <si>
+    <t xml:space="preserve">106577282</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21970613</t>
+  </si>
+  <si>
+    <t xml:space="preserve">475937095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10014407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99450731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16811236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">374452089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8711802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88058517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17913281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">399893091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7964806</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79544566</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11502326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">254905460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5184314</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49736787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11598289</t>
+  </si>
+  <si>
+    <t xml:space="preserve">264225211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4812832</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48879464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10577391</t>
+  </si>
+  <si>
+    <t xml:space="preserve">245443738</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3447394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34120574</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10976706</t>
+  </si>
+  <si>
+    <t xml:space="preserve">251365411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2342184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26105481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10100319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">236770305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2272431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25794549</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9462462</t>
+  </si>
+  <si>
+    <t xml:space="preserve">216097356</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3361488</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31580107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9078713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">226672199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3571147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34269810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9098129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">226696842</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3571308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34270777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ccaes_concat_diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ccaeo_concat_diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdcrs_concat_diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdcro_concat_diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24643</t>
+  </si>
+  <si>
+    <t xml:space="preserve">967</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: The difference in enrolid || claim id count in 2021 is because some claims have enrolids that exist in the s and o tables that do not map to any enrolid in the a or t tables</t>
   </si>
 </sst>
 </file>
@@ -883,16 +968,16 @@
         <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
@@ -900,28 +985,28 @@
         <v>2017</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="I11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12">
@@ -929,28 +1014,28 @@
         <v>2018</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="H12" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="I12" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13">
@@ -958,28 +1043,28 @@
         <v>2019</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="H13" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="I13" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14">
@@ -987,28 +1072,28 @@
         <v>2020</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="H14" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="I14" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15">
@@ -1016,33 +1101,33 @@
         <v>2021</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="H15" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="I15" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18">
@@ -1050,16 +1135,16 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19">
@@ -1067,16 +1152,16 @@
         <v>2011</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20">
@@ -1084,16 +1169,16 @@
         <v>2012</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21">
@@ -1101,16 +1186,16 @@
         <v>2013</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22">
@@ -1118,16 +1203,16 @@
         <v>2014</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23">
@@ -1135,16 +1220,16 @@
         <v>2015</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24">
@@ -1152,16 +1237,16 @@
         <v>2016</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25">
@@ -1169,16 +1254,16 @@
         <v>2017</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26">
@@ -1186,16 +1271,16 @@
         <v>2018</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="E26" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27">
@@ -1203,16 +1288,16 @@
         <v>2019</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28">
@@ -1220,16 +1305,16 @@
         <v>2020</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="E28" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29">
@@ -1237,16 +1322,629 @@
         <v>2021</v>
       </c>
       <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="10.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="17.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="17.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="17.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="17.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="17.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="17.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="17.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="17.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="9.15" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" t="s">
+        <v>99</v>
+      </c>
+      <c r="I9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B11" t="s">
         <v>105</v>
       </c>
+      <c r="C11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" t="s">
+        <v>111</v>
+      </c>
+      <c r="I12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H13" t="s">
+        <v>115</v>
+      </c>
+      <c r="I13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" t="s">
+        <v>126</v>
+      </c>
+      <c r="H15" t="s">
+        <v>127</v>
+      </c>
+      <c r="I15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B29" t="s">
+        <v>133</v>
+      </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="D29" t="s">
-        <v>107</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
-        <v>108</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>